<commit_message>
Program now automatically tracks all scores from game and writes to excel upon exiting.
</commit_message>
<xml_diff>
--- a/game/performanceData/test1.xlsx
+++ b/game/performanceData/test1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>Visit #</t>
   </si>
@@ -31,37 +31,34 @@
     <t>s0_1</t>
   </si>
   <si>
-    <t>s0_2</t>
-  </si>
-  <si>
     <t>Mean Time Spent</t>
   </si>
   <si>
     <t>s1_1</t>
   </si>
   <si>
-    <t>s1_2</t>
-  </si>
-  <si>
     <t>s2_1</t>
   </si>
   <si>
     <t>s2_2</t>
   </si>
   <si>
-    <t>s2_3</t>
-  </si>
-  <si>
-    <t>s5_1</t>
-  </si>
-  <si>
     <t>s6_1</t>
   </si>
   <si>
+    <t>s6_2</t>
+  </si>
+  <si>
     <t>s7_1</t>
   </si>
   <si>
+    <t>s7_2</t>
+  </si>
+  <si>
     <t>s8_1</t>
+  </si>
+  <si>
+    <t>s8_2</t>
   </si>
 </sst>
 </file>
@@ -421,21 +418,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3.57</v>
+        <v>0.039</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2.232</v>
-      </c>
       <c r="D3">
-        <v>2.901</v>
+        <v>0.039</v>
       </c>
     </row>
   </sheetData>
@@ -461,24 +452,18 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>1.375</v>
+        <v>6.767</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>1.308</v>
-      </c>
       <c r="D3">
-        <v>1.3415</v>
+        <v>6.767</v>
       </c>
     </row>
   </sheetData>
@@ -487,57 +472,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2.382</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>6.96</v>
-      </c>
-      <c r="D3">
-        <v>3.460333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1.039</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -555,18 +489,45 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>41.484</v>
+        <v>1.971</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2.544</v>
+      </c>
       <c r="D3">
-        <v>41.484</v>
+        <v>2.2575</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -592,18 +553,24 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>6.083</v>
+        <v>6.07</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>6.073</v>
+      </c>
       <c r="D3">
-        <v>6.083</v>
+        <v>6.0715</v>
       </c>
     </row>
   </sheetData>
@@ -629,18 +596,24 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>61.21</v>
+        <v>61.19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>61.187</v>
+      </c>
       <c r="D3">
-        <v>61.21</v>
+        <v>61.1885</v>
       </c>
     </row>
   </sheetData>
@@ -650,13 +623,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,20 +637,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>3.836</v>
+        <v>3.691</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>3.655</v>
+      </c>
       <c r="D3">
-        <v>3.836</v>
+        <v>3.673</v>
+      </c>
+      <c r="G3">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>